<commit_message>
correções dos calculos ok
</commit_message>
<xml_diff>
--- a/TODO.xlsx
+++ b/TODO.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\monteirt\Projetos_Git\tcc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\monteirt\git_projects\tcc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="34">
   <si>
     <t>Botão para calcular novo PPL depois de enviar.</t>
   </si>
@@ -125,6 +125,9 @@
   </si>
   <si>
     <t>Variaveis com o nome do tipo Xnn (no ultimo elemento trava o sistema)</t>
+  </si>
+  <si>
+    <t>Primeiro elemento com sinal negativo</t>
   </si>
 </sst>
 </file>
@@ -479,15 +482,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="60.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15">
@@ -509,7 +513,7 @@
         <v>21</v>
       </c>
       <c r="B3" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -522,17 +526,25 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="B5" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
         <v>32</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" t="s">
         <v>27</v>
       </c>
     </row>
@@ -546,7 +558,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>

</xml_diff>

<commit_message>
Mathml dos Recalculos Pronto
</commit_message>
<xml_diff>
--- a/TODO.xlsx
+++ b/TODO.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9750"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9750" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="TESTES" sheetId="3" r:id="rId1"/>
@@ -484,8 +484,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -598,8 +598,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>

</xml_diff>